<commit_message>
updated faillure retries through search
</commit_message>
<xml_diff>
--- a/zipcodes/USZIPCodes202503_Processed.xlsx
+++ b/zipcodes/USZIPCodes202503_Processed.xlsx
@@ -478,7 +478,11 @@
           <t>IL</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">

</xml_diff>

<commit_message>
restructured search results page for better processing
</commit_message>
<xml_diff>
--- a/zipcodes/USZIPCodes202503_Processed.xlsx
+++ b/zipcodes/USZIPCodes202503_Processed.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,55 +453,63 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ARCTIC VLG</t>
+          <t>Chicago</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AL</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>not found</t>
+          <t>added</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>El Paso</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>IL</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>added</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>El Paso</t>
+          <t>Los Angeles</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>TX</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Ridgewood</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>NY</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -509,12 +517,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Ridgewood</t>
+          <t>Norwalk</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -522,12 +530,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Norwalk</t>
+          <t>Katy</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>TX</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -535,12 +543,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Katy</t>
+          <t>Pacoima</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>TX</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -548,7 +556,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Pacoima</t>
+          <t>Bell Gardens</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -561,12 +569,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Bell Gardens</t>
+          <t>Bronx</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>NY</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -574,7 +582,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Bronx</t>
+          <t>Brooklyn</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -587,12 +595,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Brooklyn</t>
+          <t>Fontana</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -600,12 +608,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Brooklyn</t>
+          <t>Lakewood</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>NJ</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -639,7 +647,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Fontana</t>
+          <t>Hawthorne</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -652,12 +660,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Lakewood</t>
+          <t>Elmhurst</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NY</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -665,12 +673,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Brooklyn</t>
+          <t>Sylmar</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -678,12 +686,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Brooklyn</t>
+          <t>Long Beach</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
@@ -691,12 +699,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Hawthorne</t>
+          <t>Frisco</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>TX</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -704,12 +712,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Elmhurst</t>
+          <t>Antioch</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
@@ -717,7 +725,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Sylmar</t>
+          <t>South Gate</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -730,7 +738,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Long Beach</t>
+          <t>Los Angeles</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -743,12 +751,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Frisco</t>
+          <t>Bronx</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>TX</t>
+          <t>NY</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
@@ -756,12 +764,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Antioch</t>
+          <t>Riverside</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
@@ -769,12 +777,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>South Gate</t>
+          <t>New York</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>NY</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
@@ -782,12 +790,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Fontana</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
@@ -795,12 +803,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Brooklyn</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>NY</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
@@ -808,12 +816,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Bronx</t>
+          <t>Grand Prairie</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>TX</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
@@ -821,12 +829,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Riverside</t>
+          <t>Brooklyn</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>NY</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
@@ -834,12 +842,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>New York</t>
+          <t>Pittsburg</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
@@ -847,12 +855,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Fontana</t>
+          <t>Mckinney</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>TX</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
@@ -860,12 +868,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Brooklyn</t>
+          <t>Brownsville</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>TX</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
@@ -873,12 +881,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Grand Prairie</t>
+          <t>Brooklyn</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>TX</t>
+          <t>NY</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
@@ -886,12 +894,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Brooklyn</t>
+          <t>Westminster</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
@@ -899,12 +907,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Pittsburg</t>
+          <t>Chicago</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
@@ -912,12 +920,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Mckinney</t>
+          <t>Chicago</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>TX</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
@@ -925,12 +933,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Brownsville</t>
+          <t>Santa Ana</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>TX</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
@@ -951,12 +959,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Westminster</t>
+          <t>Staten Island</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>NY</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
@@ -964,12 +972,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Woodside</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>NY</t>
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
@@ -977,12 +985,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Lawrenceville</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>GA</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
@@ -990,7 +998,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Santa Ana</t>
+          <t>Chino</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1003,12 +1011,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Brooklyn</t>
+          <t>Sugar Land</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>TX</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
@@ -1016,12 +1024,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Staten Island</t>
+          <t>Lawrenceville</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>GA</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
@@ -1029,93 +1037,15 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Woodside</t>
+          <t>Anaheim</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>Lawrenceville</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr"/>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>Chino</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>CA</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr"/>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>Sugar Land</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>TX</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr"/>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>Lawrenceville</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr"/>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>Chicago</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>IL</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr"/>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>Anaheim</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>CA</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added mouse moves + Json save
</commit_message>
<xml_diff>
--- a/zipcodes/USZIPCodes202503_Processed.xlsx
+++ b/zipcodes/USZIPCodes202503_Processed.xlsx
@@ -512,7 +512,11 @@
           <t>NY</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -525,7 +529,11 @@
           <t>CA</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">

</xml_diff>